<commit_message>
finished simulated annealing draft
</commit_message>
<xml_diff>
--- a/Line Production December.xlsx
+++ b/Line Production December.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/GitHub/OR programming assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_264C7E0A8E251D02E61BEFD3885DE81339901F68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48B3A7F7-B73D-4559-A0F9-84969D64F66A}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_264C7E0A8E251D02E61BEFD3885DE81339901F68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFE5CE4B-B4AD-490D-AD34-38B283F2A56C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,12 +189,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -211,7 +217,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +505,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -540,13 +546,13 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>66</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>66</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>110</v>
       </c>
       <c r="E2">
@@ -572,13 +578,13 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>9</v>
       </c>
       <c r="E3">
@@ -604,13 +610,13 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
@@ -636,13 +642,13 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>6</v>
       </c>
       <c r="E5">
@@ -668,13 +674,13 @@
       <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>95</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>95</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>159</v>
       </c>
       <c r="E6">
@@ -703,10 +709,10 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
       <c r="E7">
@@ -732,13 +738,13 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>8</v>
       </c>
       <c r="E8">
@@ -764,13 +770,13 @@
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
       <c r="E9">
@@ -799,10 +805,10 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
@@ -831,10 +837,10 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
@@ -860,13 +866,13 @@
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>33</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>33</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>54</v>
       </c>
       <c r="E12">
@@ -892,13 +898,13 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
@@ -924,13 +930,13 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
@@ -956,13 +962,13 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>19</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>19</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>24</v>
       </c>
       <c r="E15">
@@ -988,13 +994,13 @@
       <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
@@ -1020,13 +1026,13 @@
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>13</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>17</v>
       </c>
       <c r="E17">
@@ -1052,13 +1058,13 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>32</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>32</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>54</v>
       </c>
       <c r="E18">
@@ -1084,13 +1090,13 @@
       <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>38</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>38</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19">
         <v>63</v>
       </c>
       <c r="E19">
@@ -1116,13 +1122,13 @@
       <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>8</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>8</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>10</v>
       </c>
       <c r="E20">
@@ -1148,13 +1154,13 @@
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
@@ -1180,13 +1186,13 @@
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>59</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>59</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>98</v>
       </c>
       <c r="E22">
@@ -1212,13 +1218,13 @@
       <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
@@ -1244,13 +1250,13 @@
       <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>66</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>66</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>111</v>
       </c>
       <c r="E24">
@@ -1276,13 +1282,13 @@
       <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>32</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>32</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25">
         <v>53</v>
       </c>
       <c r="E25">
@@ -1308,13 +1314,13 @@
       <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26">
         <v>6</v>
       </c>
       <c r="E26">
@@ -1340,13 +1346,13 @@
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>6</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>6</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27">
         <v>7</v>
       </c>
       <c r="E27">
@@ -1372,13 +1378,13 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>47</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>47</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28">
         <v>78</v>
       </c>
       <c r="E28">
@@ -1404,13 +1410,13 @@
       <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>26</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>26</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29">
         <v>33</v>
       </c>
       <c r="E29">
@@ -1436,13 +1442,13 @@
       <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>13</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>13</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30">
         <v>16</v>
       </c>
       <c r="E30">
@@ -1468,13 +1474,13 @@
       <c r="A31" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>58</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>58</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31">
         <v>96</v>
       </c>
       <c r="E31">
@@ -1500,13 +1506,13 @@
       <c r="A32" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>45</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>45</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32">
         <v>75</v>
       </c>
       <c r="E32">
@@ -1532,13 +1538,13 @@
       <c r="A33" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>28</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>28</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33">
         <v>35</v>
       </c>
       <c r="E33">
@@ -1564,13 +1570,13 @@
       <c r="A34" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>24</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>24</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34">
         <v>40</v>
       </c>
       <c r="E34">
@@ -1596,13 +1602,13 @@
       <c r="A35" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>19</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>19</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>23</v>
       </c>
       <c r="E35">
@@ -1628,13 +1634,13 @@
       <c r="A36" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
@@ -1660,13 +1666,13 @@
       <c r="A37" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>12</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>12</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>15</v>
       </c>
       <c r="E37">
@@ -1692,13 +1698,13 @@
       <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
         <v>9</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
         <v>9</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38">
         <v>11</v>
       </c>
       <c r="E38">
@@ -1724,13 +1730,13 @@
       <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
         <v>9</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>9</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39">
         <v>11</v>
       </c>
       <c r="E39">
@@ -1756,13 +1762,13 @@
       <c r="A40" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="1">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
         <v>1</v>
       </c>
       <c r="E40">
@@ -1788,13 +1794,13 @@
       <c r="A41" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41">
         <v>8</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
         <v>8</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41">
         <v>9</v>
       </c>
       <c r="E41">
@@ -1828,6 +1834,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="cc31558d369f2b18f4665515cc568258">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f1c0ceaf010dca137c910c274b4031a0" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -2030,15 +2045,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A1CB7BC-C52F-44D0-AD38-9184B592C6F5}">
   <ds:schemaRefs>
@@ -2057,6 +2063,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35C8D400-3C79-4C0A-91A1-221C0DB88FB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94A06C80-BE10-4E0C-BC2F-0B9FAA9BC96A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2073,12 +2087,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35C8D400-3C79-4C0A-91A1-221C0DB88FB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>